<commit_message>
Finish the history data table
</commit_message>
<xml_diff>
--- a/history data/history data.xlsx
+++ b/history data/history data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEW\Desktop\history-project-2022\wars and fights table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEW\Desktop\history-project-2022\history data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B3787-7B43-4319-B783-8E6EA5958AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC97E60C-D739-40ED-9A52-0F5ACEAF078D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16008" yWindow="3276" windowWidth="23040" windowHeight="12360" xr2:uid="{1336DC81-6FE4-473F-ACEF-74E2AFB55FCB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1336DC81-6FE4-473F-ACEF-74E2AFB55FCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>Битка</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>Балкански съюз(България, Сърбия, Гърция, Черна Гора) vs Османска империя</t>
+  </si>
+  <si>
+    <t>Териториално разширение и връщане на територия</t>
+  </si>
+  <si>
+    <t>Първа световна</t>
+  </si>
+  <si>
+    <t>1914-1918</t>
+  </si>
+  <si>
+    <t>Централни сили(Германия, Италия, Австро-Унгария) vs Антантата</t>
+  </si>
+  <si>
+    <t>Териториално разширение и връщане на територия(не ги получава)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -660,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5108ABBD-352D-4681-BC01-12DFE5F3F77E}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1089,6 +1107,32 @@
       <c r="D27" s="6" t="s">
         <v>79</v>
       </c>
+      <c r="E27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>